<commit_message>
double checking and rerunning with alaska state fixed
</commit_message>
<xml_diff>
--- a/data/fishery_vuln_summary.xlsx
+++ b/data/fishery_vuln_summary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lknelson\Documents\GitHub\climate_perceptions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B27D4EED-FC66-4382-BA28-9C6A396B697E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEFCC63-B5B2-452B-B21B-8E2CBF5CDD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26985" yWindow="2745" windowWidth="15375" windowHeight="11415"/>
+    <workbookView xWindow="32415" yWindow="2865" windowWidth="15375" windowHeight="11415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fishery_vuln_summary" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>fishery</t>
   </si>
@@ -105,12 +117,18 @@
   </si>
   <si>
     <t>urchin</t>
+  </si>
+  <si>
+    <t>Fishery</t>
+  </si>
+  <si>
+    <t>Dungeness crab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,7 +663,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -656,14 +674,15 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1019,16 +1038,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1059,8 +1078,23 @@
       <c r="L1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1094,8 +1128,23 @@
       <c r="L2">
         <v>0.66468253968253999</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0.672619047619048</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0.51587301587301604</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0.52380952380952395</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0.99260853199478505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1129,8 +1178,23 @@
       <c r="L3">
         <v>0.68092292906745999</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0.62008928571428601</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0.53622606449987398</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0.46701388888888901</v>
+      </c>
+      <c r="S3" s="5">
+        <v>1.0145187856356299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1164,8 +1228,23 @@
       <c r="L4">
         <v>0.86342592592592604</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0.73263888888888895</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0.421296296296296</v>
+      </c>
+      <c r="S4" s="5">
+        <v>1.09484434606767</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1199,8 +1278,23 @@
       <c r="L5">
         <v>0.70830026455026496</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0.65715811965811999</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0.50278038847117801</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0.43874643874643898</v>
+      </c>
+      <c r="S5" s="5">
+        <v>1.03197102180052</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1234,8 +1328,23 @@
       <c r="L6">
         <v>0.39351851851851799</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0.407407407407407</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0.52777777777777801</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0.869403580132458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1269,8 +1378,23 @@
       <c r="L7">
         <v>0.71746780473195504</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0.66866987179487203</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0.51077915140415098</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0.439727463312369</v>
+      </c>
+      <c r="S7" s="5">
+        <v>1.0371499655285901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1304,8 +1428,23 @@
       <c r="L8">
         <v>0.49166666666666597</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0.43333333333333302</v>
+      </c>
+      <c r="S8" s="5">
+        <v>1.13508536198204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1339,8 +1478,23 @@
       <c r="L9">
         <v>0.81690671060090703</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" s="5">
+        <v>0.72720074268239399</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0.53209012584012605</v>
+      </c>
+      <c r="R9" s="5">
+        <v>0.41815476190476197</v>
+      </c>
+      <c r="S9" s="5">
+        <v>1.1084252183673999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1374,8 +1528,23 @@
       <c r="L10">
         <v>0.81994047619047605</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0.68452380952380998</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0.52430555555555602</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0.38888888888888901</v>
+      </c>
+      <c r="S10" s="5">
+        <v>1.0681751107167501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1409,8 +1578,23 @@
       <c r="L11">
         <v>0.88266594516594599</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="5">
+        <v>0.71347402597402598</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>0.54292929292929304</v>
+      </c>
+      <c r="R11" s="5">
+        <v>0.37373737373737398</v>
+      </c>
+      <c r="S11" s="5">
+        <v>1.1112084715113599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1444,8 +1628,23 @@
       <c r="L12">
         <v>0.94883286647992604</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12" s="5">
+        <v>0.77440476190476204</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>0.55024509803921595</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0.37581699346405201</v>
+      </c>
+      <c r="S12" s="5">
+        <v>1.1573814469053501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1479,8 +1678,23 @@
       <c r="L13">
         <v>0.67938311688311603</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" s="5">
+        <v>0.60551948051948101</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0.52335858585858597</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0.449494949494949</v>
+      </c>
+      <c r="S13" s="5">
+        <v>0.99727980518796699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1514,8 +1728,23 @@
       <c r="L14">
         <v>0.62638888888888899</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0.53888888888888897</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0.96075591244060798</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>6</v>
       </c>
@@ -1802,31 +2031,32 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1834,10 +2064,10 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -1847,291 +2077,291 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>0.4375</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>0.58333330000000005</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>0.38888888999999999</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>0.95138889999999998</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>0.5</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>0.1666667</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>0.38888888999999999</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>0.80699109999999996</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>0.58333330000000005</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>0.61111110000000002</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>0.30555556</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>1.0936121999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>0.58333330000000005</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>0.4166667</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>0.58333332999999998</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>0.82915620000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>0.65</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>0.3333333</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>0.5</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>0.88521810000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>0.75</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>0.61111110000000002</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>0.55555555999999995</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>1.0646538000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>0.75</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>0.30555559999999998</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>0.25</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>1.1037954000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>0.78571429999999998</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>0.4375</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>0.47222222000000003</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>1.0427379999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>0.8125</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>0.72222220000000004</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>0.33333332999999998</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>1.2752277000000001</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>0.8125</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>0.36111110000000002</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>0.58333332999999998</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <v>0.98192089999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>0.83333330000000005</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>0.52777779999999996</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>0.30555556</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <v>1.2063362</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>0.83333330000000005</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>0.72222220000000004</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="4">
         <v>0.27777777999999997</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>1.3182012000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>0.83333330000000005</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>0.83333330000000005</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>0.33333332999999998</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="4">
         <v>1.3540064000000001</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>1</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <v>0.61111110000000002</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="4">
         <v>5.5555559999999997E-2</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="4">
         <v>1.5051352</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>1</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <v>0.88888889999999998</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="4">
         <v>0.25</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="4">
         <v>1.5338263999999999</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>1</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <v>0.22222220000000001</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="4">
         <v>0.61111110999999996</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="4">
         <v>1.0957268</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>1</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="4">
         <v>0.19444444</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="4">
         <v>1.6275501999999999</v>
       </c>
     </row>
@@ -2163,4 +2393,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA9AB6FF-A05C-4036-BDEF-27E51F23A8C9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates and checking code
</commit_message>
<xml_diff>
--- a/data/fishery_vuln_summary.xlsx
+++ b/data/fishery_vuln_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lknelson\Documents\GitHub\climate_perceptions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEFCC63-B5B2-452B-B21B-8E2CBF5CDD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EFADBF-9EB2-47B0-ABB2-487F280C3E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32415" yWindow="2865" windowWidth="15375" windowHeight="11415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fishery_vuln_summary" sheetId="1" r:id="rId1"/>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:S14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2399,7 +2399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA9AB6FF-A05C-4036-BDEF-27E51F23A8C9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>